<commit_message>
Change the milliseconds to nanoseconds and remade the tests.
</commit_message>
<xml_diff>
--- a/Comparaçoes fibonacci.xlsx
+++ b/Comparaçoes fibonacci.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://iselpt-my.sharepoint.com/personal/a47199_alunos_isel_pt/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a1904d7873b19b1d/Documentos/Universidade/AED/laboratorio1-g03/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{538B0CF0-E381-4E91-B196-9251717A0EC1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="114" documentId="8_{538B0CF0-E381-4E91-B196-9251717A0EC1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{9D9C36B6-22AB-4909-B607-8FD2575A5507}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B3DE1E32-7736-47AE-9EFB-1CF789E27A64}"/>
+    <workbookView xWindow="1905" yWindow="2055" windowWidth="21600" windowHeight="11025" xr2:uid="{B3DE1E32-7736-47AE-9EFB-1CF789E27A64}"/>
   </bookViews>
   <sheets>
     <sheet name="nº1" sheetId="9" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="5">
   <si>
     <t>Dynamic Programming</t>
   </si>
@@ -48,9 +48,6 @@
   </si>
   <si>
     <t>N</t>
-  </si>
-  <si>
-    <t>-</t>
   </si>
 </sst>
 </file>
@@ -427,7 +424,7 @@
   <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O20" sqref="O20"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -462,16 +459,16 @@
         <v>0</v>
       </c>
       <c r="B3" s="1">
-        <v>1</v>
+        <v>1.62</v>
       </c>
       <c r="C3" s="1">
-        <v>1</v>
+        <v>0.69</v>
       </c>
       <c r="D3" s="1">
-        <v>0</v>
+        <v>1.77</v>
       </c>
       <c r="E3" s="1">
-        <v>0</v>
+        <v>0.78</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -479,33 +476,29 @@
         <v>1</v>
       </c>
       <c r="B4" s="1">
-        <v>2</v>
+        <v>0.92</v>
       </c>
       <c r="C4" s="1">
-        <v>1358</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>732.28</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="1">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="C5" s="1">
-        <v>1</v>
+        <v>0.87</v>
       </c>
       <c r="D5" s="1">
-        <v>1</v>
+        <v>0.68</v>
       </c>
       <c r="E5" s="1">
-        <v>2</v>
+        <v>1.28</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -513,16 +506,16 @@
         <v>3</v>
       </c>
       <c r="B6" s="1">
-        <v>0</v>
+        <v>0.73</v>
       </c>
       <c r="C6" s="1">
-        <v>0</v>
+        <v>0.63</v>
       </c>
       <c r="D6" s="1">
-        <v>1</v>
+        <v>0.61</v>
       </c>
       <c r="E6" s="1">
-        <v>1</v>
+        <v>0.74</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -552,16 +545,16 @@
         <v>0</v>
       </c>
       <c r="B10" s="1">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="C10" s="1">
-        <v>1</v>
+        <v>0.72</v>
       </c>
       <c r="D10" s="1">
-        <v>1</v>
+        <v>2.38</v>
       </c>
       <c r="E10" s="1">
-        <v>0</v>
+        <v>0.92</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -569,33 +562,29 @@
         <v>1</v>
       </c>
       <c r="B11" s="1">
-        <v>0</v>
+        <v>0.83</v>
       </c>
       <c r="C11" s="1">
-        <v>802</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>787.74</v>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B12" s="1">
-        <v>1</v>
+        <v>0.83</v>
       </c>
       <c r="C12" s="1">
-        <v>1</v>
+        <v>2.95</v>
       </c>
       <c r="D12" s="1">
-        <v>0</v>
+        <v>0.73</v>
       </c>
       <c r="E12" s="1">
-        <v>2</v>
+        <v>9.66</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -603,16 +592,16 @@
         <v>3</v>
       </c>
       <c r="B13" s="1">
-        <v>2</v>
+        <v>0.64</v>
       </c>
       <c r="C13" s="1">
-        <v>1</v>
+        <v>0.68</v>
       </c>
       <c r="D13" s="1">
-        <v>1</v>
+        <v>0.71</v>
       </c>
       <c r="E13" s="1">
-        <v>0</v>
+        <v>0.67</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -642,16 +631,16 @@
         <v>0</v>
       </c>
       <c r="B17" s="1">
-        <v>1</v>
+        <v>1.91</v>
       </c>
       <c r="C17" s="1">
-        <v>1</v>
+        <v>0.62</v>
       </c>
       <c r="D17" s="1">
-        <v>1</v>
+        <v>1.24</v>
       </c>
       <c r="E17" s="1">
-        <v>1</v>
+        <v>1.02</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -659,33 +648,29 @@
         <v>1</v>
       </c>
       <c r="B18" s="1">
-        <v>2</v>
+        <v>0.93</v>
       </c>
       <c r="C18" s="1">
-        <v>1165</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>787.16</v>
+      </c>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B19" s="1">
-        <v>1</v>
+        <v>0.67</v>
       </c>
       <c r="C19" s="1">
-        <v>3</v>
+        <v>1.67</v>
       </c>
       <c r="D19" s="1">
-        <v>1</v>
+        <v>0.67</v>
       </c>
       <c r="E19" s="1">
-        <v>3</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -693,16 +678,16 @@
         <v>3</v>
       </c>
       <c r="B20" s="1">
-        <v>1</v>
+        <v>0.73</v>
       </c>
       <c r="C20" s="1">
-        <v>2</v>
+        <v>1.21</v>
       </c>
       <c r="D20" s="1">
-        <v>0</v>
+        <v>0.65</v>
       </c>
       <c r="E20" s="1">
-        <v>2</v>
+        <v>1.93</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -732,16 +717,16 @@
         <v>0</v>
       </c>
       <c r="B24" s="1">
-        <v>1</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="C24" s="1">
-        <v>1</v>
+        <v>0.69</v>
       </c>
       <c r="D24" s="1">
-        <v>1</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="E24" s="1">
-        <v>0</v>
+        <v>0.78</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -749,33 +734,29 @@
         <v>1</v>
       </c>
       <c r="B25" s="1">
-        <v>1</v>
+        <v>0.96</v>
       </c>
       <c r="C25" s="1">
-        <v>640</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>972.45</v>
+      </c>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B26" s="1">
-        <v>1</v>
+        <v>0.69</v>
       </c>
       <c r="C26" s="1">
-        <v>3</v>
+        <v>0.66</v>
       </c>
       <c r="D26" s="1">
         <v>1</v>
       </c>
       <c r="E26" s="1">
-        <v>1</v>
+        <v>2.2799999999999998</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -783,16 +764,16 @@
         <v>3</v>
       </c>
       <c r="B27" s="1">
-        <v>5</v>
+        <v>0.63</v>
       </c>
       <c r="C27" s="1">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="D27" s="1">
-        <v>1</v>
+        <v>0.91</v>
       </c>
       <c r="E27" s="1">
-        <v>1</v>
+        <v>1.36</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -822,16 +803,16 @@
         <v>0</v>
       </c>
       <c r="B31" s="1">
-        <v>4</v>
+        <v>0.99</v>
       </c>
       <c r="C31" s="1">
-        <v>1</v>
+        <v>0.82</v>
       </c>
       <c r="D31" s="1">
-        <v>1</v>
+        <v>0.67</v>
       </c>
       <c r="E31" s="1">
-        <v>1</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -839,33 +820,29 @@
         <v>1</v>
       </c>
       <c r="B32" s="1">
-        <v>5</v>
+        <v>0.95</v>
       </c>
       <c r="C32" s="1">
-        <v>709</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>759.38</v>
+      </c>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B33" s="1">
-        <v>1</v>
+        <v>0.77</v>
       </c>
       <c r="C33" s="1">
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="D33" s="1">
-        <v>1</v>
+        <v>1.02</v>
       </c>
       <c r="E33" s="1">
-        <v>1</v>
+        <v>1.21</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -873,16 +850,16 @@
         <v>3</v>
       </c>
       <c r="B34" s="1">
-        <v>1</v>
+        <v>0.59</v>
       </c>
       <c r="C34" s="1">
-        <v>1</v>
+        <v>0.67</v>
       </c>
       <c r="D34" s="1">
-        <v>1</v>
+        <v>3.88</v>
       </c>
       <c r="E34" s="1">
-        <v>1</v>
+        <v>0.61</v>
       </c>
     </row>
   </sheetData>
@@ -892,6 +869,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009C3B8360D724154F8D37A5F0701EA111" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1ef49ac0d3be2da6c356aa8b424d6a01">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="06286271-e381-4835-bb58-b5e5383d42c2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c07c3c004574752f49bf4e8734373a76" ns3:_="">
     <xsd:import namespace="06286271-e381-4835-bb58-b5e5383d42c2"/>
@@ -1037,22 +1029,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2E310DD3-A9FF-4C84-A1CF-66EB1AE2C3E4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6944E0E4-F347-4762-B582-985F5E25B7C4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1004653C-61F5-4493-AF2A-49BB12200A43}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1068,21 +1062,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6944E0E4-F347-4762-B582-985F5E25B7C4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2E310DD3-A9FF-4C84-A1CF-66EB1AE2C3E4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>